<commit_message>
Finished Create EC2 and Describe EC2
</commit_message>
<xml_diff>
--- a/admin/wall.xlsx
+++ b/admin/wall.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30560" windowHeight="17040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33540" windowHeight="19440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$L$3</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Priority</t>
   </si>
@@ -73,11 +76,6 @@
     <t>Specify AMI and size for EC2</t>
   </si>
   <si>
-    <t>As a SysAdmin
-I want to know the DNS name of my EC2
-So that I can remotely login and install stuffs in it</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
@@ -94,11 +92,6 @@
 So that I can install more and varied apps on it</t>
   </si>
   <si>
-    <t>Given An EC2 instance is running
-When I describe my instance
-Then I should see the DNS name</t>
-  </si>
-  <si>
     <t>Remotely run a script</t>
   </si>
   <si>
@@ -110,13 +103,71 @@
     <t>Given An existing EC2 VM
 When I remotely run a script
 Then The script should be executed on the EC2</t>
+  </si>
+  <si>
+    <t>Terminate an EC2</t>
+  </si>
+  <si>
+    <t>As a SysAdmin
+I want to terminsate a currently running EC2
+So that I do not use uneeded resources</t>
+  </si>
+  <si>
+    <t>Given An existing EC2 VM
+When I kill it
+Then The EC2 should be terminstaed</t>
+  </si>
+  <si>
+    <t>Create EC2 with custom params</t>
+  </si>
+  <si>
+    <t>As a SysAdmin
+I want to create an EC2 VM with given ami and size
+So that I can provision an adapted VM for the future installs</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>Remote</t>
+  </si>
+  <si>
+    <t>Given An existing AWS account
+When I create a new instance with ami &lt;ami&gt; and size &lt;size&gt;
+Then I should have an EC2 VM created on the Amazon cloud with the correct ami and size</t>
+  </si>
+  <si>
+    <t>Given An EC2 instance is running
+When I describe my instance
+Then I should see its details</t>
+  </si>
+  <si>
+    <t>As a SysAdmin
+I want to know the DNS Name of my EC2
+So that I can remotely login and install stuffs in it</t>
+  </si>
+  <si>
+    <t>As a SysAdmin
+I want to know the details of my EC2
+So that I can manage all my EC2s</t>
+  </si>
+  <si>
+    <t>Describe EC2 - DNS Name</t>
+  </si>
+  <si>
+    <t>Given An EC2 instance is running
+When I describe my instance for DNS name
+Then I should see its DNS name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -145,6 +196,18 @@
       <color theme="1"/>
       <name val="Wingdings 2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Wingdings 2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -163,7 +226,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -173,8 +236,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -188,16 +265,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,18 +628,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L45"/>
+  <dimension ref="B3:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="59.83203125" customWidth="1"/>
-    <col min="5" max="5" width="64.33203125" customWidth="1"/>
-    <col min="7" max="9" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="59.83203125" customWidth="1"/>
+    <col min="6" max="6" width="64.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:12">
@@ -546,15 +650,17 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1"/>
       <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
@@ -578,134 +684,172 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="2:12" ht="45">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="2:12" s="8" customFormat="1" ht="45">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4" t="s">
+      <c r="F5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="2:12" ht="62" customHeight="1">
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="2:12" ht="56" customHeight="1">
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="I6" s="4"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="2:12" ht="62" customHeight="1">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="2:12" s="8" customFormat="1" ht="62" customHeight="1">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="2:12" ht="16" customHeight="1">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="4"/>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="2:12" ht="62" customHeight="1">
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="2:12" ht="60">
+    <row r="9" spans="2:12" ht="62" customHeight="1">
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>12</v>
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="2:12" ht="45">
+    <row r="10" spans="2:12" ht="62" customHeight="1">
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="2:12">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+    <row r="11" spans="2:12" ht="60">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -713,11 +857,19 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="2:12">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+    <row r="12" spans="2:12" ht="45">
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -1078,14 +1230,30 @@
       <c r="L39" s="1"/>
     </row>
     <row r="40" spans="2:12">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
     </row>
     <row r="41" spans="2:12">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
     </row>
     <row r="42" spans="2:12">
       <c r="G42" s="4"/>
@@ -1107,7 +1275,22 @@
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
     </row>
+    <row r="46" spans="2:12">
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="2:12">
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+    </row>
   </sheetData>
+  <autoFilter ref="B3:L3">
+    <sortState ref="B6:E11">
+      <sortCondition ref="B3"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Finished create with params and describe User Stories. Changed run scenario parsing to process scenarios indenpendently
</commit_message>
<xml_diff>
--- a/admin/wall.xlsx
+++ b/admin/wall.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33540" windowHeight="19440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33540" windowHeight="19220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Priority</t>
   </si>
@@ -79,11 +79,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>Given An existing AWS account
-When I create a new instance
-Then I should have an EC2 VM created on the Amazon cloud</t>
-  </si>
-  <si>
     <t>Describe EC2</t>
   </si>
   <si>
@@ -140,27 +135,41 @@
 Then I should have an EC2 VM created on the Amazon cloud with the correct ami and size</t>
   </si>
   <si>
-    <t>Given An EC2 instance is running
-When I describe my instance
-Then I should see its details</t>
-  </si>
-  <si>
-    <t>As a SysAdmin
-I want to know the DNS Name of my EC2
-So that I can remotely login and install stuffs in it</t>
-  </si>
-  <si>
     <t>As a SysAdmin
 I want to know the details of my EC2
 So that I can manage all my EC2s</t>
   </si>
   <si>
-    <t>Describe EC2 - DNS Name</t>
-  </si>
-  <si>
-    <t>Given An EC2 instance is running
-When I describe my instance for DNS name
-Then I should see its DNS name</t>
+    <t>BDD Framework</t>
+  </si>
+  <si>
+    <t>Specify line number of feature file</t>
+  </si>
+  <si>
+    <t>Specify feature file</t>
+  </si>
+  <si>
+    <t>Given An existing AWS account
+When I create a new instance
+Then I should have an EC2 VM created on the Amazon cloud
+Given An existing AWS account
+When I create a new instance with ami &lt;ami&gt; and size &lt;size&gt;
+Then I should have an EC2 VM created on the Amazon cloud with the correct ami and size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given An EC2 instance is running
+When I describe my instance
+Then I should see its details
+Given An EC2 instance is running
+When I describe my instance DNS name
+Then I should see its DNS name
+Given An EC2 instance is running
+When I describe my instance Ami ID
+Then I should see its Ami ID
+Given An EC2 instance is running
+When I describe my instance size
+Then I should see its size
+</t>
   </si>
 </sst>
 </file>
@@ -198,14 +207,14 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="0" tint="-0.34998626667073579"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="0" tint="-0.34998626667073579"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Wingdings 2"/>
     </font>
   </fonts>
@@ -226,8 +235,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -276,7 +295,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -288,6 +307,11 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -299,6 +323,11 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -628,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L47"/>
+  <dimension ref="B3:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -639,8 +668,8 @@
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="59.83203125" customWidth="1"/>
-    <col min="6" max="6" width="64.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="69.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="13.83203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" style="3"/>
   </cols>
@@ -650,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
@@ -684,12 +713,12 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="2:12" s="8" customFormat="1" ht="45">
+    <row r="5" spans="2:12" s="8" customFormat="1" ht="138" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
@@ -698,7 +727,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -709,46 +738,46 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="2:12" ht="56" customHeight="1">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:12" s="8" customFormat="1" ht="67" customHeight="1">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="F6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="2:12" s="8" customFormat="1" ht="62" customHeight="1">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="2:12" s="8" customFormat="1" ht="240">
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -761,19 +790,19 @@
     </row>
     <row r="8" spans="2:12" ht="62" customHeight="1">
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>15</v>
@@ -786,19 +815,19 @@
     </row>
     <row r="9" spans="2:12" ht="62" customHeight="1">
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>15</v>
@@ -809,47 +838,43 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="2:12" ht="62" customHeight="1">
+    <row r="10" spans="2:12" ht="60">
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="2:12" ht="60">
+    <row r="11" spans="2:12" ht="45">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -857,19 +882,17 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="2:12" ht="45">
+    <row r="12" spans="2:12" ht="41" customHeight="1">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -878,15 +901,23 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="2:12">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+    <row r="13" spans="2:12" ht="43" customHeight="1">
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1243,17 +1274,9 @@
       <c r="L40" s="1"/>
     </row>
     <row r="41" spans="2:12">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
     </row>
     <row r="42" spans="2:12">
       <c r="G42" s="4"/>
@@ -1279,11 +1302,6 @@
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
-    </row>
-    <row r="47" spans="2:12">
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="B3:L3">

</xml_diff>

<commit_message>
Started remote install story
</commit_message>
<xml_diff>
--- a/admin/wall.xlsx
+++ b/admin/wall.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Priority</t>
   </si>
@@ -73,31 +73,13 @@
 And The Name tag should be set to my_ec2</t>
   </si>
   <si>
-    <t>Specify AMI and size for EC2</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
     <t>Describe EC2</t>
   </si>
   <si>
-    <t>As a SysAdmin
-I want to specifiy the AMI and the EC2 size when creating an EC2 VM
-So that I can install more and varied apps on it</t>
-  </si>
-  <si>
     <t>Remotely run a script</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a SysAdmin
-I want to remotely run a script on an existing EC2
-So that I can install packages on it </t>
-  </si>
-  <si>
-    <t>Given An existing EC2 VM
-When I remotely run a script
-Then The script should be executed on the EC2</t>
   </si>
   <si>
     <t>Terminate an EC2</t>
@@ -170,6 +152,16 @@
 When I describe my instance size
 Then I should see its size
 </t>
+  </si>
+  <si>
+    <t>Given An existing VM
+When I remotely run a script
+Then The script should be executed on the VM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a SysAdmin
+I want to remotely run a script on an existing VM
+So that I can install packages on it </t>
   </si>
 </sst>
 </file>
@@ -657,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L46"/>
+  <dimension ref="B3:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -679,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
@@ -718,7 +710,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
@@ -727,12 +719,12 @@
         <v>8</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -743,21 +735,21 @@
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -768,21 +760,21 @@
         <v>9</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -793,19 +785,19 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -818,19 +810,19 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -843,7 +835,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
@@ -861,7 +853,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="2:12" ht="45">
+    <row r="11" spans="2:12" ht="41" customHeight="1">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
@@ -869,11 +861,9 @@
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -882,42 +872,36 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="2:12" ht="41" customHeight="1">
+    <row r="12" spans="2:12" ht="43" customHeight="1">
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="2:12" ht="43" customHeight="1">
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>33</v>
-      </c>
+    <row r="13" spans="2:12">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="I13" s="4"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1261,17 +1245,9 @@
       <c r="L39" s="1"/>
     </row>
     <row r="40" spans="2:12">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
     </row>
     <row r="41" spans="2:12">
       <c r="G41" s="4"/>
@@ -1297,11 +1273,6 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
-    </row>
-    <row r="46" spans="2:12">
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="B3:L3">

</xml_diff>